<commit_message>
Clean up stupid colour structs and implement patterns (class 0x06). Now, you can select taskbar items and some lines draw. Replace some multiplications with shifts.
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C11F76-938F-48DF-8A6B-538403A0C191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD65FC19-50D2-4F95-BFF2-0622B2C72CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Code cleanup</t>
   </si>
   <si>
-    <t>Seems fine, always check for bugs</t>
-  </si>
-  <si>
     <t>Maybe done, verify!</t>
   </si>
   <si>
@@ -315,13 +312,25 @@
   </si>
   <si>
     <t>Random Blits end up in the middle of the screen?!</t>
+  </si>
+  <si>
+    <t>Seems fine, ALWAYS CHECK FOR BUGS</t>
+  </si>
+  <si>
+    <t>There is special hardware support, but it just renders anyway using Class 011? At least emulate starting pos</t>
+  </si>
+  <si>
+    <t>AGP broken</t>
+  </si>
+  <si>
+    <t>ZX broken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,8 +357,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +406,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -405,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -416,6 +436,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,13 +754,13 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +784,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,7 +792,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +800,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +832,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,8 +903,8 @@
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>33</v>
+      <c r="B19" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +952,7 @@
         <v>54</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +960,7 @@
         <v>55</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,7 +968,7 @@
         <v>56</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,7 +994,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,14 +1013,16 @@
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1007,7 +1030,7 @@
         <v>65</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1029,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1046,12 +1069,12 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1076,22 +1099,32 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1128,10 +1161,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,7 +1393,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1368,15 +1401,15 @@
         <v>27</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1384,7 +1417,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1392,39 +1425,39 @@
         <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIFO optimisation, hitches down to ~1-2 seconds from 5 seconds, 70% speed idle at desktop
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD65FC19-50D2-4F95-BFF2-0622B2C72CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC835E86-5BC7-40FB-99E4-5D3860BD9E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>ZX broken</t>
+  </si>
+  <si>
+    <t>It does at least partially work, but some junk gets sent to the top of the screen</t>
   </si>
 </sst>
 </file>
@@ -753,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A719D13-329D-4889-84DA-9B41795DED3E}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,8 +826,8 @@
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
+      <c r="B9" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -895,8 +898,8 @@
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>33</v>
+      <c r="B18" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
partially working text acceleration, looks inverted(??)
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC835E86-5BC7-40FB-99E4-5D3860BD9E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB19D5A4-8A48-4C3C-A292-B9D2FFEF98E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="100">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>It does at least partially work, but some junk gets sent to the top of the screen</t>
+  </si>
+  <si>
+    <t>Sometimes there are spurious rectangles at 90 degrees to the valid ones (WHAT???)</t>
   </si>
 </sst>
 </file>
@@ -756,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A719D13-329D-4889-84DA-9B41795DED3E}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1055,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1128,6 +1131,11 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove even more redundant GDI-D code
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB19D5A4-8A48-4C3C-A292-B9D2FFEF98E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F09539-C469-4FB1-825B-7A422DD6AF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -83,9 +83,6 @@
     <t>SORTA WORKING (very screwed up rendering)</t>
   </si>
   <si>
-    <t>Bugs - last updated 22 March 2025</t>
-  </si>
-  <si>
     <t>8bpp doesn't do crap</t>
   </si>
   <si>
@@ -330,6 +327,12 @@
   </si>
   <si>
     <t>Sometimes there are spurious rectangles at 90 degrees to the valid ones (WHAT???)</t>
+  </si>
+  <si>
+    <t>GDI-D: "Active Desktop Recovery" text screwed up</t>
+  </si>
+  <si>
+    <t>Bugs - last updated 24 March 2025</t>
   </si>
 </sst>
 </file>
@@ -771,13 +774,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -787,267 +790,267 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="1"/>
     </row>
@@ -1058,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1072,69 +1075,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1172,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,13 +1265,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1274,7 +1282,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1285,7 +1293,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1296,7 +1304,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>5</v>
@@ -1310,7 +1318,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1401,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1401,74 +1409,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Legitimately I don't even know how i mostly fixed it. What's going on?
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F09539-C469-4FB1-825B-7A422DD6AF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE9700A-91A4-4668-B6F7-400330091F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -329,10 +329,16 @@
     <t>Sometimes there are spurious rectangles at 90 degrees to the valid ones (WHAT???)</t>
   </si>
   <si>
-    <t>GDI-D: "Active Desktop Recovery" text screwed up</t>
-  </si>
-  <si>
     <t>Bugs - last updated 24 March 2025</t>
+  </si>
+  <si>
+    <t>GDI-D *OR* S2SB: "Active Desktop Recovery" text screwed up</t>
+  </si>
+  <si>
+    <t>S2SB: Is it set up same as GDI endianness wise?</t>
+  </si>
+  <si>
+    <t>GDI-D: Rightmost horizontal line missing when size_in=0x0010</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1075,7 +1081,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>88</v>
@@ -1143,7 +1149,17 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix 32bpp bsod by actually creating framebuffer mappings. Don't remap memory if it's 0 (prevents trashing the low/real-mode memory map), general code simplification (some things were enabled 3 times what
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE9700A-91A4-4668-B6F7-400330091F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B24434-B16A-4C2C-B2D7-EC8FE4E24C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="3285" yWindow="2325" windowWidth="28800" windowHeight="10560" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>GDI-D: Rightmost horizontal line missing when size_in=0x0010</t>
+  </si>
+  <si>
+    <t>1bpp expanded bitblit issues</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1162,6 +1165,11 @@
         <v>102</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1172,7 +1180,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A16" sqref="A15:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Redirect all PRMCIO/PRMVIO writes to SVGA subsystem, not just a few random ones.
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B24434-B16A-4C2C-B2D7-EC8FE4E24C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B955E2-AA82-42DD-BF46-14D01ACCA953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="2325" windowWidth="28800" windowHeight="10560" activeTab="1" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
   <si>
     <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
   </si>
@@ -239,9 +239,6 @@
     <t>The beta factor is not used</t>
   </si>
   <si>
-    <t>The chroma key set is not tested</t>
-  </si>
-  <si>
     <t>Some fixed, there are probably still bugs</t>
   </si>
   <si>
@@ -329,9 +326,6 @@
     <t>Sometimes there are spurious rectangles at 90 degrees to the valid ones (WHAT???)</t>
   </si>
   <si>
-    <t>Bugs - last updated 24 March 2025</t>
-  </si>
-  <si>
     <t>GDI-D *OR* S2SB: "Active Desktop Recovery" text screwed up</t>
   </si>
   <si>
@@ -341,14 +335,29 @@
     <t>GDI-D: Rightmost horizontal line missing when size_in=0x0010</t>
   </si>
   <si>
-    <t>1bpp expanded bitblit issues</t>
+    <t>GDI-E 1bpp expanded bitblit issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed </t>
+  </si>
+  <si>
+    <t>32bpp looks incredibly fucked up</t>
+  </si>
+  <si>
+    <t>Bugs - last updated 26 March 2025</t>
+  </si>
+  <si>
+    <t>Context Switching, RAMFC</t>
+  </si>
+  <si>
+    <t>GDI-A fine, GDI-D mostly good, GDI-E/1bpp colour-expanded bitblt fucked up, GDI-B and C not implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +386,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -443,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -455,6 +470,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A719D13-329D-4889-84DA-9B41795DED3E}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,15 +826,15 @@
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>69</v>
+      <c r="B6" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -842,7 +858,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -850,7 +866,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -889,8 +905,8 @@
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
+      <c r="B15" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,7 +930,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +938,7 @@
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,7 +994,7 @@
         <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -986,82 +1002,108 @@
         <v>55</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>71</v>
+        <v>105</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>94</v>
+        <v>61</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>72</v>
+        <v>62</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B39" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1070,29 +1112,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="82.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1117,57 +1160,66 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1204,10 +1256,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1436,7 +1488,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1444,15 +1496,15 @@
         <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1460,7 +1512,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1468,39 +1520,39 @@
         <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make 2k and 9x live happily together, seems vtrace register bit 1 controls rowoffset shifting
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B955E2-AA82-42DD-BF46-14D01ACCA953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B6B2DC-BFAA-42A3-8B1F-A6A43CDA816C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
-  <si>
-    <t>Resolution Testing - RIVA 128 (very very early v0.6)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>Result</t>
   </si>
@@ -212,9 +209,6 @@
     <t>Notifier Engine</t>
   </si>
   <si>
-    <t>Cleanup code</t>
-  </si>
-  <si>
     <t>Dumb Framebuffer (DFB)</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>Unify position/size structs</t>
   </si>
   <si>
-    <t>Code cleanup</t>
-  </si>
-  <si>
     <t>Maybe done, verify!</t>
   </si>
   <si>
@@ -311,9 +302,6 @@
     <t>Seems fine, ALWAYS CHECK FOR BUGS</t>
   </si>
   <si>
-    <t>There is special hardware support, but it just renders anyway using Class 011? At least emulate starting pos</t>
-  </si>
-  <si>
     <t>AGP broken</t>
   </si>
   <si>
@@ -351,13 +339,40 @@
   </si>
   <si>
     <t>GDI-A fine, GDI-D mostly good, GDI-E/1bpp colour-expanded bitblt fucked up, GDI-B and C not implemented</t>
+  </si>
+  <si>
+    <t>Enough for win9x, but no memory to memory formatting actually done</t>
+  </si>
+  <si>
+    <t>NEEDS MORE TESTING</t>
+  </si>
+  <si>
+    <t>Detection fixed, missing M2MF implementation fixed - now working in 32bpp, 16bpp has issues</t>
+  </si>
+  <si>
+    <t>Still blackscreening, not spewing garbage all over the screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detection fixed </t>
+  </si>
+  <si>
+    <t>Win9x and NT 16bpp clocking different</t>
+  </si>
+  <si>
+    <t>Needed for 9x, not for NT (uses Class 0x11)</t>
+  </si>
+  <si>
+    <t>Code cleanup/refactor</t>
+  </si>
+  <si>
+    <t>Resolution Testing - RIVA 128 (pre-v0.9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,14 +404,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +454,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -458,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -470,7 +485,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A719D13-329D-4889-84DA-9B41795DED3E}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,13 +815,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -815,291 +831,286 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>32</v>
+        <v>110</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>71</v>
+        <v>62</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="B39" s="12"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -1112,114 +1123,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="82.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="91" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="11"/>
+        <v>99</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1231,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8478C62-8A9B-4C7D-BD96-FA6577DC482D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A15:A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1247,154 +1277,154 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
         <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
+      <c r="D10" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
         <v>32</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
+      <c r="D11" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>25</v>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1">
         <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1421,29 +1451,29 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1477,82 +1507,82 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1565,7 +1595,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Split up logs into two verbosity levels (one is just init/invalid regs/object submission/pci, everything else is verbose_only)
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B6B2DC-BFAA-42A3-8B1F-A6A43CDA816C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9869DFF1-765F-4FD7-96D5-D351ED6A941F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="0" yWindow="2325" windowWidth="28800" windowHeight="10560" activeTab="4" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
   <si>
     <t>Result</t>
   </si>
@@ -308,9 +308,6 @@
     <t>ZX broken</t>
   </si>
   <si>
-    <t>It does at least partially work, but some junk gets sent to the top of the screen</t>
-  </si>
-  <si>
     <t>Sometimes there are spurious rectangles at 90 degrees to the valid ones (WHAT???)</t>
   </si>
   <si>
@@ -338,18 +335,9 @@
     <t>Context Switching, RAMFC</t>
   </si>
   <si>
-    <t>GDI-A fine, GDI-D mostly good, GDI-E/1bpp colour-expanded bitblt fucked up, GDI-B and C not implemented</t>
-  </si>
-  <si>
-    <t>Enough for win9x, but no memory to memory formatting actually done</t>
-  </si>
-  <si>
     <t>NEEDS MORE TESTING</t>
   </si>
   <si>
-    <t>Detection fixed, missing M2MF implementation fixed - now working in 32bpp, 16bpp has issues</t>
-  </si>
-  <si>
     <t>Still blackscreening, not spewing garbage all over the screen</t>
   </si>
   <si>
@@ -366,6 +354,24 @@
   </si>
   <si>
     <t>Resolution Testing - RIVA 128 (pre-v0.9)</t>
+  </si>
+  <si>
+    <t>Probably fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soft reset causes a black screen on win2k </t>
+  </si>
+  <si>
+    <t>Detection fixed, dummy M2MF implementation now working in 16/32bpp, 8bpp has issues</t>
+  </si>
+  <si>
+    <t>GDI-A, GDI-B, GDI-C, GDI-D and GDI-E seem fine, ALWAYS CHECK FOR BUGS</t>
+  </si>
+  <si>
+    <t>At least partially works, but some bugs definitely exist…</t>
+  </si>
+  <si>
+    <t>Notifications work. M2MF not actually done.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A719D13-329D-4889-84DA-9B41795DED3E}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,8 +927,8 @@
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>102</v>
+      <c r="B15" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +936,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -946,7 +952,7 @@
         <v>45</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,7 +1053,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>31</v>
@@ -1063,7 +1069,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>68</v>
@@ -1082,7 +1088,7 @@
         <v>60</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED3B20-D807-4FBF-859D-2504CFB10989}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1144,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>84</v>
@@ -1159,7 +1165,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1177,7 +1183,7 @@
         <v>83</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1185,15 +1191,15 @@
         <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1216,40 +1222,57 @@
         <v>91</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1261,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8478C62-8A9B-4C7D-BD96-FA6577DC482D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1277,7 +1300,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1388,7 +1411,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1399,7 +1422,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1494,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F705335-7801-4118-892D-11B2A198EDD8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix framebuffer size with vertical resolution > 1024 by applying large screen bit even in NV mode
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9869DFF1-765F-4FD7-96D5-D351ED6A941F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A84A884-99EA-4038-BC8D-D3490BDC4B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2325" windowWidth="28800" windowHeight="10560" activeTab="4" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
+    <workbookView xWindow="0" yWindow="4080" windowWidth="28800" windowHeight="10560" activeTab="2" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
   <si>
     <t>Result</t>
   </si>
@@ -77,9 +77,6 @@
     <t>1280x1024</t>
   </si>
   <si>
-    <t>SORTA WORKING (very screwed up rendering)</t>
-  </si>
-  <si>
     <t>8bpp doesn't do crap</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>1600x1200</t>
   </si>
   <si>
-    <t>BSOD nv3_mini+0x164c3</t>
-  </si>
-  <si>
     <t>VESA: DOOM is broken</t>
   </si>
   <si>
@@ -368,10 +362,10 @@
     <t>GDI-A, GDI-B, GDI-C, GDI-D and GDI-E seem fine, ALWAYS CHECK FOR BUGS</t>
   </si>
   <si>
-    <t>At least partially works, but some bugs definitely exist…</t>
-  </si>
-  <si>
     <t>Notifications work. M2MF not actually done.</t>
+  </si>
+  <si>
+    <t>Buffer to buffer - fine. Between buffers - not so much…</t>
   </si>
 </sst>
 </file>
@@ -809,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A719D13-329D-4889-84DA-9B41795DED3E}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,13 +815,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -837,282 +831,282 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1144,135 +1138,135 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1284,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8478C62-8A9B-4C7D-BD96-FA6577DC482D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1294,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1309,10 +1303,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1388,19 +1382,19 @@
       <c r="C8" s="1">
         <v>16</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>15</v>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>19</v>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1411,7 +1405,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1422,7 +1416,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1447,7 +1441,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1517,7 +1511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F705335-7801-4118-892D-11B2A198EDD8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1524,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1538,74 +1532,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get rid of useless "reserved" stuff and also implement 8bpp indexed mode using CLUT.
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/status.xlsx
+++ b/doc/nvidia_notes/status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A84A884-99EA-4038-BC8D-D3490BDC4B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC243D0-EC07-43D1-8D4C-4442BE734285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4080" windowWidth="28800" windowHeight="10560" activeTab="2" xr2:uid="{9BA00B2F-E35A-4F70-9E92-F85456AB4F07}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="111">
   <si>
     <t>Result</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Boulderoid v1.15</t>
   </si>
   <si>
-    <t>BSOD win32k+13c692 (CHECK CALLSTACK)</t>
-  </si>
-  <si>
     <t>DOOM</t>
   </si>
   <si>
@@ -329,9 +326,6 @@
     <t>Context Switching, RAMFC</t>
   </si>
   <si>
-    <t>NEEDS MORE TESTING</t>
-  </si>
-  <si>
     <t>Still blackscreening, not spewing garbage all over the screen</t>
   </si>
   <si>
@@ -366,6 +360,9 @@
   </si>
   <si>
     <t>Buffer to buffer - fine. Between buffers - not so much…</t>
+  </si>
+  <si>
+    <t>BSOD on reboot, but works switching to it?</t>
   </si>
 </sst>
 </file>
@@ -815,13 +812,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -831,282 +828,282 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,15 +1135,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1159,7 +1156,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1174,99 +1171,99 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1279,7 +1276,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1291,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1303,10 +1300,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1393,8 +1390,8 @@
       <c r="C9" s="1">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
+      <c r="D9" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1404,8 +1401,8 @@
       <c r="C10" s="1">
         <v>32</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>99</v>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1415,8 +1412,8 @@
       <c r="C11" s="1">
         <v>32</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>99</v>
+      <c r="D11" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1440,8 +1437,8 @@
       <c r="C13" s="1">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>22</v>
+      <c r="D13" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1535,71 +1532,71 @@
         <v>21</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>